<commit_message>
new pets: Treasure Goblin and Dread Hatchling
</commit_message>
<xml_diff>
--- a/BreedsPerPet.xlsx
+++ b/BreedsPerPet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="973" count="6857">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="977" count="6863">
   <si>
     <t>SpeciesId</t>
   </si>
@@ -2933,6 +2933,18 @@
   </si>
   <si>
     <t>inv_mace_1h_pandung_c_01</t>
+  </si>
+  <si>
+    <t>Treasure Goblin</t>
+  </si>
+  <si>
+    <t>ability_racial_packhobgoblin</t>
+  </si>
+  <si>
+    <t>Dread Hatchling</t>
+  </si>
+  <si>
+    <t>ability_mount_pandarenphoenix_green</t>
   </si>
 </sst>
 </file>
@@ -3009,7 +3021,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <sheetPr codeName="BreedsPerPet"/>
-  <dimension ref="A1:K2282"/>
+  <dimension ref="A1:K2284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -82934,6 +82946,76 @@
         <v>254</v>
       </c>
     </row>
+    <row r="2284" spans="1:11">
+      <c r="A2284" s="1">
+        <v>1365</v>
+      </c>
+      <c r="B2284" s="3">
+        <v>9</v>
+      </c>
+      <c r="C2284" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2284" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="E2284" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="F2284" s="0">
+        <v>8.90</v>
+      </c>
+      <c r="G2284" s="0">
+        <v>8.00</v>
+      </c>
+      <c r="H2284" s="0">
+        <v>8.90</v>
+      </c>
+      <c r="I2284" s="1">
+        <v>1546</v>
+      </c>
+      <c r="J2284" s="1">
+        <v>260</v>
+      </c>
+      <c r="K2284" s="1">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:11">
+      <c r="A2285" s="1">
+        <v>1386</v>
+      </c>
+      <c r="B2285" s="4">
+        <v>14</v>
+      </c>
+      <c r="C2285" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2285" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="E2285" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="F2285" s="0">
+        <v>8.12</v>
+      </c>
+      <c r="G2285" s="0">
+        <v>10.38</v>
+      </c>
+      <c r="H2285" s="0">
+        <v>7.50</v>
+      </c>
+      <c r="I2285" s="1">
+        <v>1420</v>
+      </c>
+      <c r="J2285" s="1">
+        <v>337</v>
+      </c>
+      <c r="K2285" s="1">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>